<commit_message>
added keywords in entries3
</commit_message>
<xml_diff>
--- a/carezoom_frontend/entries3.xlsx
+++ b/carezoom_frontend/entries3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinabear/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinabear/carezoom_frontend/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="165">
   <si>
     <t>title</t>
   </si>
@@ -655,6 +655,12 @@
   <si>
     <t>hepatitis</t>
   </si>
+  <si>
+    <t>medicare</t>
+  </si>
+  <si>
+    <t>integration</t>
+  </si>
 </sst>
 </file>
 
@@ -1215,7 +1221,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM3" sqref="AM3"/>
+      <selection pane="bottomLeft" activeCell="AM5" sqref="AM5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1587,7 +1593,7 @@
         <v>86</v>
       </c>
       <c r="AM3" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
@@ -1697,7 +1703,9 @@
       <c r="AL4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="AM4" s="3"/>
+      <c r="AM4" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3"/>
       <c r="AQ4" s="3"/>
@@ -1796,7 +1804,9 @@
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
-      <c r="AM5" s="3"/>
+      <c r="AM5" s="3" t="s">
+        <v>164</v>
+      </c>
       <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
       <c r="AP5" s="3"/>

</xml_diff>

<commit_message>
changed keywords to searchterm float
</commit_message>
<xml_diff>
--- a/carezoom_frontend/entries3.xlsx
+++ b/carezoom_frontend/entries3.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="400">
   <si>
     <t>Tag/Filter</t>
   </si>
@@ -1543,6 +1543,9 @@
   <si>
     <t>hepatitis C financial Incentive appointment attendance no show rate</t>
   </si>
+  <si>
+    <t>Search Terms</t>
+  </si>
 </sst>
 </file>
 
@@ -2074,7 +2077,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2211,7 +2214,9 @@
         <v>108</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="31" t="s">
+        <v>399</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>39</v>
       </c>

</xml_diff>